<commit_message>
KiCAD files and other added
</commit_message>
<xml_diff>
--- a/A320 Boards.xlsx
+++ b/A320 Boards.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\KiCad\#MSFS2020\Hardware\Boards\A320\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\MSFS2020\Boards\A320-PCBs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12E66DCF-5378-4DD7-BC9D-6DE142CC7328}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CE20746-EA8F-4E45-BF48-2B29D4C50737}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7665" yWindow="405" windowWidth="39645" windowHeight="20700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12135" yWindow="300" windowWidth="38055" windowHeight="20700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Board status" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1013" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1017" uniqueCount="297">
   <si>
     <t>Board</t>
   </si>
@@ -145,9 +145,6 @@
   </si>
   <si>
     <t>Mega 2560</t>
-  </si>
-  <si>
-    <t>NA</t>
   </si>
   <si>
     <t>???</t>
@@ -1725,7 +1722,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W2" sqref="W2:W61"/>
+      <selection pane="bottomLeft" activeCell="T12" sqref="T12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1778,15 +1775,15 @@
         <v>11</v>
       </c>
       <c r="K1" s="9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="L1" s="9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="M1" s="9"/>
       <c r="N1" s="9"/>
       <c r="O1" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="P1" s="11" t="s">
         <v>10</v>
@@ -1830,19 +1827,19 @@
         <v>8</v>
       </c>
       <c r="K2" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="L2" s="9" t="s">
         <v>176</v>
-      </c>
-      <c r="L2" s="9" t="s">
-        <v>177</v>
       </c>
       <c r="M2" s="9" t="s">
         <v>9</v>
       </c>
       <c r="N2" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="O2" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P2" s="11" t="s">
         <v>8</v>
@@ -1860,13 +1857,13 @@
         <v>35</v>
       </c>
       <c r="U2" s="22" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="V2" s="22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="W2" s="36" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
@@ -1936,7 +1933,7 @@
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C4" s="14" t="s">
         <v>4</v>
@@ -1999,7 +1996,7 @@
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C5" s="14" t="s">
         <v>4</v>
@@ -2062,7 +2059,7 @@
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C6" s="14" t="s">
         <v>4</v>
@@ -2125,7 +2122,7 @@
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C7" s="14" t="s">
         <v>4</v>
@@ -2188,7 +2185,7 @@
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C8" s="14" t="s">
         <v>4</v>
@@ -2251,7 +2248,7 @@
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C9" s="14" t="s">
         <v>4</v>
@@ -2314,7 +2311,7 @@
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C10" s="14" t="s">
         <v>4</v>
@@ -2377,7 +2374,7 @@
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B11" s="65" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C11" s="23"/>
       <c r="D11" s="23"/>
@@ -2414,7 +2411,7 @@
         <v>4</v>
       </c>
       <c r="W11" s="35" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
@@ -2450,12 +2447,12 @@
         <v>36</v>
       </c>
       <c r="W12" s="35" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C13" s="23"/>
       <c r="D13" s="23"/>
@@ -2496,12 +2493,12 @@
         <v>4</v>
       </c>
       <c r="W13" s="35" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:23" ht="90" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C14" s="23"/>
       <c r="D14" s="23"/>
@@ -2532,7 +2529,7 @@
         <v>36</v>
       </c>
       <c r="W14" s="35" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
@@ -2657,7 +2654,7 @@
     </row>
     <row r="19" spans="1:23" ht="105" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C19" s="23"/>
       <c r="D19" s="23"/>
@@ -2688,7 +2685,7 @@
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C20" s="14"/>
       <c r="D20" s="14"/>
@@ -2719,12 +2716,12 @@
         <v>36</v>
       </c>
       <c r="W20" s="35" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C21" s="23"/>
       <c r="D21" s="23"/>
@@ -2765,12 +2762,12 @@
         <v>4</v>
       </c>
       <c r="W21" s="35" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:23" ht="90" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C22" s="23"/>
       <c r="D22" s="23"/>
@@ -2801,7 +2798,7 @@
         <v>36</v>
       </c>
       <c r="W22" s="35" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.25">
@@ -2834,7 +2831,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C24" s="23"/>
       <c r="D24" s="23"/>
@@ -2867,7 +2864,7 @@
     </row>
     <row r="25" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C25" s="23"/>
       <c r="D25" s="23"/>
@@ -2920,7 +2917,7 @@
         <v>4</v>
       </c>
       <c r="W25" s="63" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.25">
@@ -2958,7 +2955,7 @@
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C27" s="62"/>
       <c r="D27" s="62"/>
@@ -3024,7 +3021,7 @@
     </row>
     <row r="29" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C29" s="23"/>
       <c r="D29" s="23"/>
@@ -3077,12 +3074,12 @@
         <v>4</v>
       </c>
       <c r="W29" s="63" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C30" s="23"/>
       <c r="D30" s="23"/>
@@ -3109,6 +3106,9 @@
       <c r="Q30" s="27"/>
       <c r="R30" s="28"/>
       <c r="S30" s="28"/>
+      <c r="T30" s="21" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A31" s="59"/>
@@ -3140,7 +3140,7 @@
         <v>26</v>
       </c>
       <c r="B32" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C32" s="23" t="s">
         <v>4</v>
@@ -3171,10 +3171,13 @@
       <c r="Q32" s="27"/>
       <c r="R32" s="28"/>
       <c r="S32" s="28"/>
+      <c r="T32" s="21" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C33" s="23" t="s">
         <v>4</v>
@@ -3239,7 +3242,7 @@
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B34" s="4" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C34" s="23" t="s">
         <v>4</v>
@@ -3332,12 +3335,12 @@
       <c r="R35" s="28"/>
       <c r="S35" s="28"/>
       <c r="T35" s="21" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="36" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C36" s="23"/>
       <c r="D36" s="23"/>
@@ -3366,7 +3369,7 @@
     </row>
     <row r="37" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B37" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C37" s="23" t="s">
         <v>4</v>
@@ -3431,7 +3434,7 @@
     </row>
     <row r="38" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B38" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C38" s="23" t="s">
         <v>4</v>
@@ -3496,7 +3499,7 @@
     </row>
     <row r="39" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B39" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C39" s="23" t="s">
         <v>4</v>
@@ -3561,7 +3564,7 @@
     </row>
     <row r="40" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C40" s="23"/>
       <c r="D40" s="23"/>
@@ -3588,6 +3591,9 @@
       <c r="Q40" s="27"/>
       <c r="R40" s="28"/>
       <c r="S40" s="28"/>
+      <c r="T40" s="21" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="41" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A41" s="59"/>
@@ -3645,7 +3651,7 @@
       <c r="R42" s="28"/>
       <c r="S42" s="28"/>
       <c r="T42" s="21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="43" spans="1:23" x14ac:dyDescent="0.25">
@@ -3680,7 +3686,7 @@
     </row>
     <row r="44" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B44" s="4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C44" s="23" t="s">
         <v>4</v>
@@ -3745,7 +3751,7 @@
     </row>
     <row r="45" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C45" s="23"/>
       <c r="D45" s="23"/>
@@ -3786,12 +3792,12 @@
         <v>4</v>
       </c>
       <c r="W45" s="35" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="46" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C46" s="23"/>
       <c r="D46" s="23"/>
@@ -3820,10 +3826,13 @@
       <c r="S46" s="28" t="s">
         <v>4</v>
       </c>
+      <c r="T46" s="21" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="47" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C47" s="23"/>
       <c r="D47" s="23"/>
@@ -3860,7 +3869,7 @@
         <v>4</v>
       </c>
       <c r="W47" s="35" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="48" spans="1:23" x14ac:dyDescent="0.25">
@@ -3896,7 +3905,7 @@
         <v>36</v>
       </c>
       <c r="W48" s="35" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="49" spans="2:23" x14ac:dyDescent="0.25">
@@ -3955,10 +3964,10 @@
         <v>4</v>
       </c>
       <c r="T49" s="21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="W49" s="35" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="50" spans="2:23" x14ac:dyDescent="0.25">
@@ -3992,12 +4001,12 @@
         <v>36</v>
       </c>
       <c r="W50" s="35" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="51" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B51" s="4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C51" s="23" t="s">
         <v>4</v>
@@ -4060,12 +4069,12 @@
         <v>4</v>
       </c>
       <c r="W51" s="35" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="52" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C52" s="23"/>
       <c r="D52" s="23"/>
@@ -4106,7 +4115,7 @@
         <v>4</v>
       </c>
       <c r="W52" s="35" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="53" spans="2:23" x14ac:dyDescent="0.25">
@@ -4148,7 +4157,7 @@
     </row>
     <row r="54" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B54" s="4" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C54" s="29" t="s">
         <v>4</v>
@@ -4213,7 +4222,7 @@
     </row>
     <row r="55" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B55" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C55" s="29" t="s">
         <v>4</v>
@@ -4278,7 +4287,7 @@
     </row>
     <row r="56" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B56" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C56" s="29" t="s">
         <v>4</v>
@@ -4343,7 +4352,7 @@
     </row>
     <row r="57" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B57" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C57" s="29" t="s">
         <v>4</v>
@@ -4408,7 +4417,7 @@
     </row>
     <row r="58" spans="2:23" ht="30" x14ac:dyDescent="0.25">
       <c r="B58" s="64" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C58" s="29" t="s">
         <v>4</v>
@@ -4473,7 +4482,7 @@
     </row>
     <row r="59" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B59" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C59" s="29" t="s">
         <v>4</v>
@@ -4538,7 +4547,7 @@
     </row>
     <row r="60" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B60" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C60" s="29" t="s">
         <v>4</v>
@@ -4603,7 +4612,7 @@
     </row>
     <row r="61" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B61" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C61" s="29" t="s">
         <v>4</v>
@@ -4695,154 +4704,154 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>221</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>237</v>
+      </c>
+      <c r="B4" t="s">
         <v>238</v>
-      </c>
-      <c r="B4" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>240</v>
+      </c>
+      <c r="B5" t="s">
         <v>241</v>
-      </c>
-      <c r="B5" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>252</v>
+      </c>
+      <c r="B7" t="s">
         <v>253</v>
-      </c>
-      <c r="B7" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B9" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B10" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B12" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B13" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>243</v>
+      </c>
+      <c r="B15" t="s">
         <v>244</v>
-      </c>
-      <c r="B15" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B16" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>246</v>
+      </c>
+      <c r="B17" t="s">
         <v>247</v>
-      </c>
-      <c r="B17" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B19" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B20" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>233</v>
+      </c>
+      <c r="B22" t="s">
         <v>234</v>
-      </c>
-      <c r="B22" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>235</v>
+      </c>
+      <c r="B23" t="s">
         <v>236</v>
-      </c>
-      <c r="B23" t="s">
-        <v>237</v>
       </c>
     </row>
   </sheetData>
@@ -4929,139 +4938,139 @@
   <sheetData>
     <row r="1" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A1" s="42" t="s">
+        <v>178</v>
+      </c>
+      <c r="B1" s="42" t="s">
         <v>179</v>
       </c>
-      <c r="B1" s="42" t="s">
-        <v>180</v>
-      </c>
       <c r="C1" s="42" t="s">
+        <v>178</v>
+      </c>
+      <c r="D1" s="42" t="s">
         <v>179</v>
       </c>
-      <c r="D1" s="42" t="s">
-        <v>180</v>
-      </c>
       <c r="E1" s="42" t="s">
+        <v>178</v>
+      </c>
+      <c r="F1" s="42" t="s">
         <v>179</v>
       </c>
-      <c r="F1" s="42" t="s">
-        <v>180</v>
-      </c>
       <c r="G1" s="42" t="s">
+        <v>178</v>
+      </c>
+      <c r="H1" s="42" t="s">
         <v>179</v>
       </c>
-      <c r="H1" s="42" t="s">
-        <v>180</v>
-      </c>
       <c r="I1" s="42" t="s">
+        <v>178</v>
+      </c>
+      <c r="J1" s="42" t="s">
         <v>179</v>
       </c>
-      <c r="J1" s="42" t="s">
-        <v>180</v>
-      </c>
       <c r="K1" s="42" t="s">
+        <v>178</v>
+      </c>
+      <c r="L1" s="42" t="s">
         <v>179</v>
       </c>
-      <c r="L1" s="42" t="s">
-        <v>180</v>
-      </c>
       <c r="M1" s="42" t="s">
+        <v>178</v>
+      </c>
+      <c r="N1" s="42" t="s">
         <v>179</v>
       </c>
-      <c r="N1" s="42" t="s">
-        <v>180</v>
-      </c>
       <c r="O1" s="42" t="s">
+        <v>178</v>
+      </c>
+      <c r="P1" s="42" t="s">
         <v>179</v>
       </c>
-      <c r="P1" s="42" t="s">
-        <v>180</v>
-      </c>
       <c r="Q1" s="42" t="s">
+        <v>178</v>
+      </c>
+      <c r="R1" s="42" t="s">
         <v>179</v>
       </c>
-      <c r="R1" s="42" t="s">
-        <v>180</v>
-      </c>
       <c r="S1" s="42" t="s">
+        <v>178</v>
+      </c>
+      <c r="T1" s="42" t="s">
         <v>179</v>
       </c>
-      <c r="T1" s="42" t="s">
-        <v>180</v>
-      </c>
       <c r="U1" s="42" t="s">
+        <v>178</v>
+      </c>
+      <c r="V1" s="42" t="s">
         <v>179</v>
       </c>
-      <c r="V1" s="42" t="s">
-        <v>180</v>
-      </c>
       <c r="W1" s="42" t="s">
+        <v>178</v>
+      </c>
+      <c r="X1" s="42" t="s">
         <v>179</v>
       </c>
-      <c r="X1" s="42" t="s">
-        <v>180</v>
-      </c>
       <c r="Y1" s="42" t="s">
+        <v>178</v>
+      </c>
+      <c r="Z1" s="42" t="s">
         <v>179</v>
       </c>
-      <c r="Z1" s="42" t="s">
-        <v>180</v>
-      </c>
       <c r="AA1" s="42" t="s">
+        <v>178</v>
+      </c>
+      <c r="AB1" s="42" t="s">
         <v>179</v>
       </c>
-      <c r="AB1" s="42" t="s">
-        <v>180</v>
-      </c>
       <c r="AC1" s="42" t="s">
+        <v>178</v>
+      </c>
+      <c r="AD1" s="42" t="s">
         <v>179</v>
       </c>
-      <c r="AD1" s="42" t="s">
-        <v>180</v>
-      </c>
       <c r="AE1" s="42" t="s">
+        <v>178</v>
+      </c>
+      <c r="AF1" s="42" t="s">
         <v>179</v>
       </c>
-      <c r="AF1" s="42" t="s">
-        <v>180</v>
-      </c>
       <c r="AG1" s="42" t="s">
+        <v>178</v>
+      </c>
+      <c r="AH1" s="42" t="s">
         <v>179</v>
       </c>
-      <c r="AH1" s="42" t="s">
-        <v>180</v>
-      </c>
       <c r="AI1" s="42" t="s">
+        <v>178</v>
+      </c>
+      <c r="AJ1" s="42" t="s">
         <v>179</v>
       </c>
-      <c r="AJ1" s="42" t="s">
-        <v>180</v>
-      </c>
       <c r="AK1" s="42" t="s">
+        <v>178</v>
+      </c>
+      <c r="AL1" s="42" t="s">
         <v>179</v>
       </c>
-      <c r="AL1" s="42" t="s">
-        <v>180</v>
-      </c>
       <c r="AM1" s="42" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="2" spans="1:40" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="47"/>
       <c r="B2" s="50" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C2" s="47"/>
       <c r="D2" s="51" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E2" s="47"/>
       <c r="F2" s="50" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G2" s="47"/>
       <c r="H2" s="43" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I2" s="47"/>
       <c r="J2" s="43" t="s">
@@ -5069,66 +5078,66 @@
       </c>
       <c r="K2" s="47"/>
       <c r="L2" s="43" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M2" s="47"/>
       <c r="N2" s="43" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="O2" s="47"/>
       <c r="P2" s="43" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="Q2" s="47"/>
       <c r="R2" s="43" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="S2" s="47"/>
       <c r="T2" s="43" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="U2" s="47"/>
       <c r="V2" s="43" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="W2" s="47"/>
       <c r="X2" s="52" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="Y2" s="47"/>
       <c r="Z2" s="51" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AA2" s="47"/>
       <c r="AB2" s="53" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AC2" s="47"/>
       <c r="AD2" s="53" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AE2" s="47"/>
       <c r="AF2" s="49" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AG2" s="39"/>
       <c r="AH2" s="58" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="AI2" s="39"/>
       <c r="AJ2" s="58" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="AK2" s="39"/>
       <c r="AL2" s="58" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="AM2" s="39"/>
     </row>
     <row r="3" spans="1:40" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="47"/>
       <c r="B3" s="56" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C3" s="47"/>
       <c r="D3" s="49"/>
@@ -5136,65 +5145,65 @@
       <c r="F3" s="49"/>
       <c r="G3" s="47"/>
       <c r="H3" s="49" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I3" s="47"/>
       <c r="J3" s="49" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K3" s="47"/>
       <c r="L3" s="49"/>
       <c r="M3" s="47"/>
       <c r="N3" s="54" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="O3" s="47"/>
       <c r="P3" s="54" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="Q3" s="47"/>
       <c r="R3" s="54" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="S3" s="47"/>
       <c r="T3" s="50" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="U3" s="47"/>
       <c r="V3" s="49" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="W3" s="47"/>
       <c r="X3" s="52" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y3" s="47"/>
       <c r="Z3" s="51" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AA3" s="47"/>
       <c r="AB3" s="55" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="AC3" s="47"/>
       <c r="AD3" s="55" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AE3" s="47"/>
       <c r="AF3" s="43" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="AG3" s="39"/>
       <c r="AH3" s="50" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="AI3" s="39"/>
       <c r="AJ3" s="50" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="AK3" s="39"/>
       <c r="AL3" s="50" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="AM3" s="39"/>
     </row>
@@ -5302,209 +5311,209 @@
     </row>
     <row r="6" spans="1:40" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H6" t="s">
+        <v>161</v>
+      </c>
+      <c r="J6" t="s">
+        <v>165</v>
+      </c>
+      <c r="L6" t="s">
+        <v>113</v>
+      </c>
+      <c r="N6" t="s">
+        <v>154</v>
+      </c>
+      <c r="P6" t="s">
+        <v>135</v>
+      </c>
+      <c r="R6" t="s">
+        <v>142</v>
+      </c>
+      <c r="T6" t="s">
+        <v>167</v>
+      </c>
+      <c r="V6" t="s">
+        <v>207</v>
+      </c>
+      <c r="X6" t="s">
+        <v>161</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>161</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>161</v>
+      </c>
+      <c r="AD6" t="s">
         <v>162</v>
       </c>
-      <c r="J6" t="s">
+      <c r="AF6" t="s">
         <v>166</v>
       </c>
-      <c r="L6" t="s">
-        <v>114</v>
-      </c>
-      <c r="N6" t="s">
-        <v>155</v>
-      </c>
-      <c r="P6" t="s">
-        <v>136</v>
-      </c>
-      <c r="R6" t="s">
-        <v>143</v>
-      </c>
-      <c r="T6" t="s">
-        <v>168</v>
-      </c>
-      <c r="V6" t="s">
-        <v>208</v>
-      </c>
-      <c r="X6" t="s">
-        <v>162</v>
-      </c>
-      <c r="Z6" t="s">
-        <v>162</v>
-      </c>
-      <c r="AB6" t="s">
-        <v>162</v>
-      </c>
-      <c r="AD6" t="s">
-        <v>163</v>
-      </c>
-      <c r="AF6" t="s">
-        <v>167</v>
-      </c>
       <c r="AH6" t="s">
+        <v>210</v>
+      </c>
+      <c r="AJ6" t="s">
         <v>211</v>
       </c>
-      <c r="AJ6" t="s">
+      <c r="AL6" t="s">
         <v>212</v>
-      </c>
-      <c r="AL6" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="7" spans="1:40" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="J7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="R7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="T7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="V7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="X7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="Z7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="8" spans="1:40" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="L8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="T8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="9" spans="1:40" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="10" spans="1:40" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="14" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A14" s="41" t="s">
+        <v>178</v>
+      </c>
+      <c r="B14" s="42" t="s">
         <v>179</v>
       </c>
-      <c r="B14" s="42" t="s">
-        <v>180</v>
-      </c>
       <c r="C14" s="42" t="s">
+        <v>178</v>
+      </c>
+      <c r="D14" s="42" t="s">
         <v>179</v>
       </c>
-      <c r="D14" s="42" t="s">
-        <v>180</v>
-      </c>
       <c r="E14" s="42" t="s">
+        <v>178</v>
+      </c>
+      <c r="F14" s="42" t="s">
         <v>179</v>
       </c>
-      <c r="F14" s="42" t="s">
-        <v>180</v>
-      </c>
       <c r="G14" s="42" t="s">
+        <v>178</v>
+      </c>
+      <c r="H14" s="42" t="s">
         <v>179</v>
       </c>
-      <c r="H14" s="42" t="s">
-        <v>180</v>
-      </c>
       <c r="I14" s="42" t="s">
+        <v>178</v>
+      </c>
+      <c r="J14" s="42" t="s">
         <v>179</v>
       </c>
-      <c r="J14" s="42" t="s">
-        <v>180</v>
-      </c>
       <c r="K14" s="42" t="s">
+        <v>178</v>
+      </c>
+      <c r="L14" s="42" t="s">
         <v>179</v>
       </c>
-      <c r="L14" s="42" t="s">
-        <v>180</v>
-      </c>
       <c r="M14" s="42" t="s">
+        <v>178</v>
+      </c>
+      <c r="N14" s="42" t="s">
         <v>179</v>
       </c>
-      <c r="N14" s="42" t="s">
-        <v>180</v>
-      </c>
       <c r="O14" s="42" t="s">
+        <v>178</v>
+      </c>
+      <c r="P14" s="42" t="s">
         <v>179</v>
       </c>
-      <c r="P14" s="42" t="s">
-        <v>180</v>
-      </c>
       <c r="Q14" s="42" t="s">
+        <v>178</v>
+      </c>
+      <c r="R14" s="42" t="s">
         <v>179</v>
       </c>
-      <c r="R14" s="42" t="s">
-        <v>180</v>
-      </c>
       <c r="S14" s="42" t="s">
+        <v>178</v>
+      </c>
+      <c r="T14" s="42" t="s">
         <v>179</v>
       </c>
-      <c r="T14" s="42" t="s">
-        <v>180</v>
-      </c>
       <c r="U14" s="42" t="s">
+        <v>178</v>
+      </c>
+      <c r="V14" s="42" t="s">
         <v>179</v>
       </c>
-      <c r="V14" s="42" t="s">
-        <v>180</v>
-      </c>
       <c r="W14" s="42" t="s">
+        <v>178</v>
+      </c>
+      <c r="X14" s="42" t="s">
         <v>179</v>
       </c>
-      <c r="X14" s="42" t="s">
-        <v>180</v>
-      </c>
       <c r="Y14" s="42" t="s">
+        <v>178</v>
+      </c>
+      <c r="Z14" s="42" t="s">
         <v>179</v>
       </c>
-      <c r="Z14" s="42" t="s">
-        <v>180</v>
-      </c>
       <c r="AA14" s="42" t="s">
+        <v>178</v>
+      </c>
+      <c r="AB14" s="42" t="s">
         <v>179</v>
       </c>
-      <c r="AB14" s="42" t="s">
-        <v>180</v>
-      </c>
       <c r="AC14" s="42" t="s">
+        <v>178</v>
+      </c>
+      <c r="AD14" s="42" t="s">
         <v>179</v>
       </c>
-      <c r="AD14" s="42" t="s">
-        <v>180</v>
-      </c>
       <c r="AE14" s="42" t="s">
+        <v>178</v>
+      </c>
+      <c r="AF14" s="42" t="s">
         <v>179</v>
-      </c>
-      <c r="AF14" s="42" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="15" spans="1:40" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5512,43 +5521,43 @@
       <c r="B15" s="49"/>
       <c r="C15" s="45"/>
       <c r="D15" s="46" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E15" s="47"/>
       <c r="F15" s="43" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G15" s="47"/>
       <c r="H15" s="43" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I15" s="47"/>
       <c r="J15" s="49" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K15" s="47"/>
       <c r="L15" s="48"/>
       <c r="M15" s="47"/>
       <c r="N15" s="43" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="O15" s="47"/>
       <c r="P15" s="46" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="Q15" s="47"/>
       <c r="R15" s="46" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="S15" s="47"/>
       <c r="T15" s="49"/>
       <c r="U15" s="47"/>
       <c r="V15" s="43" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="W15" s="47"/>
       <c r="X15" s="49" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="Y15" s="47"/>
       <c r="Z15" s="49"/>
@@ -5556,77 +5565,77 @@
       <c r="AB15" s="49"/>
       <c r="AC15" s="47"/>
       <c r="AD15" s="49" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="AE15" s="47"/>
       <c r="AF15" s="43" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:40" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="38"/>
       <c r="B16" s="54" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C16" s="45"/>
       <c r="D16" s="54" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E16" s="47"/>
       <c r="F16" s="54" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G16" s="47"/>
       <c r="H16" s="54" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I16" s="47"/>
       <c r="J16" s="54" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K16" s="47"/>
       <c r="L16" s="44" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M16" s="47"/>
       <c r="N16" s="44" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O16" s="47"/>
       <c r="P16" s="44" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="Q16" s="47"/>
       <c r="R16" s="44" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="S16" s="47"/>
       <c r="T16" s="55" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="U16" s="47"/>
       <c r="V16" s="43" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="W16" s="47"/>
       <c r="X16" s="49" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="Y16" s="47"/>
       <c r="Z16" s="49" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AA16" s="47"/>
       <c r="AB16" s="54" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AC16" s="47"/>
       <c r="AD16" s="54" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AE16" s="47"/>
       <c r="AF16" s="54" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="17" spans="1:34" x14ac:dyDescent="0.25">
@@ -5717,52 +5726,52 @@
     </row>
     <row r="19" spans="1:34" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
+        <v>118</v>
+      </c>
+      <c r="D19" t="s">
+        <v>144</v>
+      </c>
+      <c r="F19" t="s">
+        <v>111</v>
+      </c>
+      <c r="H19" t="s">
+        <v>129</v>
+      </c>
+      <c r="J19" t="s">
+        <v>123</v>
+      </c>
+      <c r="L19" t="s">
         <v>119</v>
       </c>
-      <c r="D19" t="s">
-        <v>145</v>
-      </c>
-      <c r="F19" t="s">
+      <c r="N19" t="s">
+        <v>150</v>
+      </c>
+      <c r="P19" t="s">
+        <v>148</v>
+      </c>
+      <c r="R19" t="s">
+        <v>170</v>
+      </c>
+      <c r="T19" t="s">
+        <v>163</v>
+      </c>
+      <c r="V19" t="s">
+        <v>161</v>
+      </c>
+      <c r="X19" t="s">
+        <v>161</v>
+      </c>
+      <c r="Z19" t="s">
+        <v>157</v>
+      </c>
+      <c r="AB19" t="s">
+        <v>160</v>
+      </c>
+      <c r="AD19" t="s">
         <v>112</v>
       </c>
-      <c r="H19" t="s">
-        <v>130</v>
-      </c>
-      <c r="J19" t="s">
-        <v>124</v>
-      </c>
-      <c r="L19" t="s">
-        <v>120</v>
-      </c>
-      <c r="N19" t="s">
-        <v>151</v>
-      </c>
-      <c r="P19" t="s">
-        <v>149</v>
-      </c>
-      <c r="R19" t="s">
-        <v>171</v>
-      </c>
-      <c r="T19" t="s">
-        <v>164</v>
-      </c>
-      <c r="V19" t="s">
-        <v>162</v>
-      </c>
-      <c r="X19" t="s">
-        <v>162</v>
-      </c>
-      <c r="Z19" t="s">
-        <v>158</v>
-      </c>
-      <c r="AB19" t="s">
-        <v>161</v>
-      </c>
-      <c r="AD19" t="s">
-        <v>113</v>
-      </c>
       <c r="AF19" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="AH19" s="57">
         <f>SUM(AH4:AN18)</f>
@@ -5771,253 +5780,253 @@
     </row>
     <row r="20" spans="1:34" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L20" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="N20" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="P20" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="R20" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="T20" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="V20" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="X20" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="AB20" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="AF20" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="21" spans="1:34" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L21" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="N21" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="R21" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="AB21" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AF21" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="22" spans="1:34" x14ac:dyDescent="0.25">
       <c r="L22" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="N22" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="AB22" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="AF22" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="23" spans="1:34" x14ac:dyDescent="0.25">
       <c r="N23" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="AB23" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AF23" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="24" spans="1:34" x14ac:dyDescent="0.25">
       <c r="AB24" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="AF24" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="25" spans="1:34" x14ac:dyDescent="0.25">
       <c r="AF25" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="26" spans="1:34" x14ac:dyDescent="0.25">
       <c r="AF26" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="27" spans="1:34" x14ac:dyDescent="0.25">
       <c r="D27" s="40"/>
       <c r="AF27" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="28" spans="1:34" x14ac:dyDescent="0.25">
       <c r="AF28" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="29" spans="1:34" x14ac:dyDescent="0.25">
       <c r="AF29" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="30" spans="1:34" x14ac:dyDescent="0.25">
       <c r="AF30" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="31" spans="1:34" x14ac:dyDescent="0.25">
       <c r="AF31" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="32" spans="1:34" x14ac:dyDescent="0.25">
       <c r="AF32" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="33" spans="32:32" x14ac:dyDescent="0.25">
       <c r="AF33" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="34" spans="32:32" x14ac:dyDescent="0.25">
       <c r="AF34" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="35" spans="32:32" x14ac:dyDescent="0.25">
       <c r="AF35" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="36" spans="32:32" x14ac:dyDescent="0.25">
       <c r="AF36" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="37" spans="32:32" x14ac:dyDescent="0.25">
       <c r="AF37" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="38" spans="32:32" x14ac:dyDescent="0.25">
       <c r="AF38" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="39" spans="32:32" x14ac:dyDescent="0.25">
       <c r="AF39" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="40" spans="32:32" x14ac:dyDescent="0.25">
       <c r="AF40" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="41" spans="32:32" x14ac:dyDescent="0.25">
       <c r="AF41" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="42" spans="32:32" x14ac:dyDescent="0.25">
       <c r="AF42" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="43" spans="32:32" x14ac:dyDescent="0.25">
       <c r="AF43" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="44" spans="32:32" x14ac:dyDescent="0.25">
       <c r="AF44" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="45" spans="32:32" x14ac:dyDescent="0.25">
       <c r="AF45" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="46" spans="32:32" x14ac:dyDescent="0.25">
       <c r="AF46" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="47" spans="32:32" x14ac:dyDescent="0.25">
       <c r="AF47" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="48" spans="32:32" x14ac:dyDescent="0.25">
       <c r="AF48" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="49" spans="32:32" x14ac:dyDescent="0.25">
       <c r="AF49" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="50" spans="32:32" x14ac:dyDescent="0.25">
       <c r="AF50" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="51" spans="32:32" x14ac:dyDescent="0.25">
       <c r="AF51" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="52" spans="32:32" x14ac:dyDescent="0.25">
       <c r="AF52" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="53" spans="32:32" x14ac:dyDescent="0.25">
       <c r="AF53" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="54" spans="32:32" x14ac:dyDescent="0.25">
       <c r="AF54" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="55" spans="32:32" x14ac:dyDescent="0.25">
       <c r="AF55" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="56" spans="32:32" x14ac:dyDescent="0.25">
       <c r="AF56" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="57" spans="32:32" x14ac:dyDescent="0.25">
       <c r="AF57" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -6044,120 +6053,120 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C1" s="37" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C2" s="37" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" t="s">
         <v>65</v>
-      </c>
-      <c r="C4" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" t="s">
         <v>67</v>
-      </c>
-      <c r="C5" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C8" t="s">
         <v>71</v>
-      </c>
-      <c r="C8" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" t="s">
         <v>54</v>
       </c>
-      <c r="B10" t="s">
-        <v>55</v>
-      </c>
       <c r="C10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
+        <v>73</v>
+      </c>
+      <c r="C15" t="s">
         <v>74</v>
-      </c>
-      <c r="C15" t="s">
-        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>